<commit_message>
Prob. 169 - dead end #3
</commit_message>
<xml_diff>
--- a/Problems/Problem 169 Seq. Analysis.xlsx
+++ b/Problems/Problem 169 Seq. Analysis.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>factors</t>
   </si>
@@ -55,12 +55,39 @@
   </si>
   <si>
     <t>diff</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0101</t>
+  </si>
+  <si>
+    <t>11001</t>
+  </si>
+  <si>
+    <t>111001</t>
+  </si>
+  <si>
+    <t>11001101</t>
+  </si>
+  <si>
+    <t>1011001001</t>
+  </si>
+  <si>
+    <t>Ternary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.000000E+00"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -90,15 +117,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -237,7 +271,17 @@
   <c:lang val="en-US"/>
   <c:chart>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.2929270727678519E-2"/>
+          <c:y val="5.1400554097404488E-2"/>
+          <c:w val="0.65714439799159108"/>
+          <c:h val="0.8326195683872849"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:ser>
@@ -253,8 +297,13 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.3515293890023805E-2"/>
+                  <c:y val="-5.1042578011081946E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000000" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
@@ -359,16 +408,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -705,15 +754,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="8" max="8" width="11.53125" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -735,160 +788,221 @@
       <c r="G1" t="s">
         <v>0</v>
       </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <f>LOG(A2)</f>
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>2</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>2</v>
       </c>
+      <c r="H2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>10</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <f t="shared" ref="B3:B7" si="0">LOG(A3)</f>
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <f>C3-C2</f>
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>5</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="2">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>100</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>19</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <f t="shared" ref="D4:D7" si="1">C4-C3</f>
         <v>14</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>19</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>20</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="H4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="2">
+        <v>201</v>
+      </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>1000</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>39</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>40</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="H5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1110</v>
+      </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>10000</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>205</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <f t="shared" si="1"/>
         <v>166</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>206</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="5">
         <v>2103</v>
       </c>
+      <c r="H6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="2">
+        <v>21121</v>
+      </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>100000</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>713</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <f t="shared" si="1"/>
         <v>508</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>714</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H7">
-        <f>714/2/3/7</f>
-        <v>17</v>
-      </c>
+      <c r="H7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="2">
+        <v>222102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="K9" s="1">
+        <f>1.171494*EXP(1.27735*25)</f>
+        <v>86574796643930.375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="K10" s="1">
+        <f>1.171494*EXP(1.27735*6)</f>
+        <v>2495.8380843015575</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="K11" s="1">
+        <f>1.171494*EXP(1.27735*5)</f>
+        <v>695.7774526851091</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="K12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
End of quest for 169 for now - uncomplete
</commit_message>
<xml_diff>
--- a/Problems/Problem 169 Seq. Analysis.xlsx
+++ b/Problems/Problem 169 Seq. Analysis.xlsx
@@ -439,15 +439,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>271462</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:colOff>257174</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>309562</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>